<commit_message>
[fixes] - minor adjustments to the data file in `template/` directory to improve performance. - fixed failed unit tests
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-data.xlsx
+++ b/template/nexial-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\nexial-core\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4D5852-A8B1-6542-8E07-69F7FEC0612B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADABB6C-A09B-4C95-AE89-C45C230C256D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,12 +134,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FFA9B7C6"/>
       <name val="Courier New"/>
       <family val="1"/>
     </font>
@@ -187,7 +181,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -199,23 +193,11 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -261,19 +243,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <color theme="1"/>
@@ -306,6 +275,19 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -598,690 +580,368 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA200"/>
+  <dimension ref="A1:AAA99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="52" width="21.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="53" max="16384" width="10.7109375" style="2" collapsed="1"/>
+    <col min="1" max="1" width="34.8984375" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.296875" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="21.296875" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="703" width="10.69921875" style="2"/>
+    <col min="704" max="16384" width="10.69921875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="HA1" s="3"/>
-      <c r="AAA1" s="3"/>
-    </row>
-    <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="HA2" s="3"/>
-      <c r="AAA2" s="3"/>
-    </row>
-    <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="HA3" s="3"/>
-      <c r="AAA3" s="3"/>
-    </row>
-    <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="HA4" s="6"/>
-      <c r="AAA4" s="7"/>
-    </row>
-    <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="HA5" s="6"/>
-      <c r="AAA5" s="7"/>
-    </row>
-    <row r="6" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="HA6" s="6"/>
-      <c r="AAA6" s="7"/>
-    </row>
-    <row r="7" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="HA7" s="6"/>
-      <c r="AAA7" s="7"/>
-    </row>
-    <row r="8" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="HA8" s="6"/>
-      <c r="AAA8" s="7"/>
-    </row>
-    <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="HA9" s="6"/>
-      <c r="AAA9" s="7"/>
-    </row>
-    <row r="10" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="HA10" s="6"/>
-      <c r="AAA10" s="7"/>
-    </row>
-    <row r="11" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
-    </row>
-    <row r="100" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-    </row>
-    <row r="101" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-    </row>
-    <row r="102" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-    </row>
-    <row r="103" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-    </row>
-    <row r="104" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-    </row>
-    <row r="105" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-    </row>
-    <row r="106" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-    </row>
-    <row r="107" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-    </row>
-    <row r="108" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-    </row>
-    <row r="109" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-    </row>
-    <row r="110" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-    </row>
-    <row r="111" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-    </row>
-    <row r="112" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-    </row>
-    <row r="113" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-    </row>
-    <row r="114" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-    </row>
-    <row r="115" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-    </row>
-    <row r="116" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-    </row>
-    <row r="117" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-    </row>
-    <row r="118" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-    </row>
-    <row r="119" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
-    </row>
-    <row r="120" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
-    </row>
-    <row r="121" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
-    </row>
-    <row r="122" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
-    </row>
-    <row r="123" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
-    </row>
-    <row r="124" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
-    </row>
-    <row r="125" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
-    </row>
-    <row r="126" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
-    </row>
-    <row r="127" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1"/>
-    </row>
-    <row r="128" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1"/>
-    </row>
-    <row r="130" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1"/>
-    </row>
-    <row r="131" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
-    </row>
-    <row r="132" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
-    </row>
-    <row r="133" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1"/>
-    </row>
-    <row r="134" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1"/>
-    </row>
-    <row r="135" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
-    </row>
-    <row r="136" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
-    </row>
-    <row r="137" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1"/>
-    </row>
-    <row r="139" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1"/>
-    </row>
-    <row r="140" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="1"/>
-    </row>
-    <row r="141" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
-    </row>
-    <row r="142" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="1"/>
-    </row>
-    <row r="143" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="1"/>
-    </row>
-    <row r="144" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="1"/>
-    </row>
-    <row r="145" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1"/>
-    </row>
-    <row r="146" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="1"/>
-    </row>
-    <row r="147" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="1"/>
-    </row>
-    <row r="148" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="1"/>
-    </row>
-    <row r="149" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="1"/>
-    </row>
-    <row r="150" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="1"/>
-    </row>
-    <row r="151" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="1"/>
-    </row>
-    <row r="152" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="1"/>
-    </row>
-    <row r="153" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
-    </row>
-    <row r="154" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="1"/>
-    </row>
-    <row r="155" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="1"/>
-    </row>
-    <row r="156" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="1"/>
-    </row>
-    <row r="157" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="1"/>
-    </row>
-    <row r="158" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="1"/>
-    </row>
-    <row r="159" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
-    </row>
-    <row r="160" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="1"/>
-    </row>
-    <row r="161" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="1"/>
-    </row>
-    <row r="162" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1"/>
-    </row>
-    <row r="163" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="1"/>
-    </row>
-    <row r="164" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="1"/>
-    </row>
-    <row r="165" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="1"/>
-    </row>
-    <row r="166" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="1"/>
-    </row>
-    <row r="167" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="1"/>
-    </row>
-    <row r="168" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="1"/>
-    </row>
-    <row r="169" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="1"/>
-    </row>
-    <row r="170" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="1"/>
-    </row>
-    <row r="171" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="1"/>
-    </row>
-    <row r="172" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="1"/>
-    </row>
-    <row r="173" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="1"/>
-    </row>
-    <row r="174" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="1"/>
-    </row>
-    <row r="175" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="1"/>
-    </row>
-    <row r="176" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="1"/>
-    </row>
-    <row r="177" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="1"/>
-    </row>
-    <row r="178" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="1"/>
-    </row>
-    <row r="179" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="1"/>
-    </row>
-    <row r="180" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="1"/>
-    </row>
-    <row r="181" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="1"/>
-    </row>
-    <row r="182" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="1"/>
-    </row>
-    <row r="183" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="1"/>
-    </row>
-    <row r="184" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="1"/>
-    </row>
-    <row r="185" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="1"/>
-    </row>
-    <row r="186" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="1"/>
-    </row>
-    <row r="187" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="1"/>
-    </row>
-    <row r="188" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="1"/>
-    </row>
-    <row r="190" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="1"/>
-    </row>
-    <row r="192" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="1"/>
-    </row>
-    <row r="193" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="1"/>
-    </row>
-    <row r="194" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="1"/>
-    </row>
-    <row r="195" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="1"/>
-    </row>
-    <row r="196" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="1"/>
-    </row>
-    <row r="197" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="1"/>
-    </row>
-    <row r="198" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="1"/>
-    </row>
-    <row r="199" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="1"/>
-    </row>
-    <row r="200" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="5" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="3" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:AZ1048576">
+  <conditionalFormatting sqref="B1:E1048576">
     <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>

</xml_diff>

<commit_message>
- added draft doc. for WebEZ
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-data.xlsx
+++ b/template/nexial-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="12645" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12585" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -55,7 +55,16 @@
     <t>1500</t>
   </si>
   <si>
-    <t>nexial.web.alwaysWait</t>
+    <t>nexial.browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>nexial.web.explicitWait</t>
+  </si>
+  <si>
+    <t>nexial.screenshotOnError</t>
   </si>
   <si>
     <t>nexial.openResult</t>
@@ -66,12 +75,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -97,58 +106,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,8 +135,97 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -172,14 +234,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,39 +248,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,31 +265,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +409,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,139 +433,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,11 +474,44 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,15 +546,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -514,15 +563,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -531,162 +571,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -711,7 +742,7 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -719,46 +750,48 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Check Cell" xfId="8" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17"/>
-    <cellStyle name="Note" xfId="10" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="11" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="12" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="13" builtinId="35"/>
-    <cellStyle name="Title" xfId="14" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="15" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="17" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="18" builtinId="19"/>
-    <cellStyle name="Input" xfId="19" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="20" builtinId="40"/>
-    <cellStyle name="Good" xfId="21" builtinId="26"/>
-    <cellStyle name="Output" xfId="22" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="23" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="24" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="25" builtinId="24"/>
-    <cellStyle name="Total" xfId="26" builtinId="25"/>
-    <cellStyle name="Bad" xfId="27" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="29" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="30" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="31" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="33" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="34" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="35" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="37" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="38" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="39" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="40" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="42" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="43" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="44" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="45" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="46" builtinId="52"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1119,10 +1152,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>
@@ -1162,22 +1195,32 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" ht="23.1" customHeight="1" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A7" s="4"/>
+    <row r="6" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" ht="23.1" customHeight="1" spans="1:1">
       <c r="A8" s="4"/>
@@ -1448,6 +1491,12 @@
     </row>
     <row r="97" ht="23.1" customHeight="1" spans="1:1">
       <c r="A97" s="4"/>
+    </row>
+    <row r="98" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A98" s="4"/>
+    </row>
+    <row r="99" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A99" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>

</xml_diff>